<commit_message>
add floats benchmark and chart
</commit_message>
<xml_diff>
--- a/images/2024-05-sep/sep-ncsvperf-workstation-vs-server-gc.xlsx
+++ b/images/2024-05-sep/sep-ncsvperf-workstation-vs-server-gc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\oss\nietras.github.io\images\2024-05-sep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB988ED1-CA1C-4E06-8E65-B213DCEB8BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B743E243-5175-4472-90FC-9F46881CF281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" xr2:uid="{C7E08072-B203-4866-8CD1-1DD39C8665B2}"/>
   </bookViews>
@@ -3965,23 +3965,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="76e46cd0-ee24-4c53-a711-52f49eba2f27" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004884246C8B9E9D49A9E87510AD9E12A5" ma:contentTypeVersion="7" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="84c6454fb2b6791ebdf2972fe509330f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="76e46cd0-ee24-4c53-a711-52f49eba2f27" xmlns:ns4="590ffc2b-f7c7-44dd-9bc9-c42f557ab722" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a35026c4dc72b333964d7c666a3013b2" ns3:_="" ns4:_="">
     <xsd:import namespace="76e46cd0-ee24-4c53-a711-52f49eba2f27"/>
@@ -4164,32 +4147,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B2F9D36-745B-47AA-BDD1-FEF14CF4623B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="76e46cd0-ee24-4c53-a711-52f49eba2f27"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="590ffc2b-f7c7-44dd-9bc9-c42f557ab722"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0E97434-C1DD-4F60-8584-0E7EBD7778AE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="76e46cd0-ee24-4c53-a711-52f49eba2f27" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A93EFB46-DEBB-48C3-9F6C-E7F9C2F08ED2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4206,4 +4181,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0E97434-C1DD-4F60-8584-0E7EBD7778AE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B2F9D36-745B-47AA-BDD1-FEF14CF4623B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="76e46cd0-ee24-4c53-a711-52f49eba2f27"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="590ffc2b-f7c7-44dd-9bc9-c42f557ab722"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>